<commit_message>
Rename UC5 from Viatris EyeCare to Eye Care Franchise
Remove company-specific branding for discretion. All Viatris
references in UC5 replaced with generic "Eye Care Franchise"
across engine, Streamlit page, Excel export, and README.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/exports/Ophthalmology_Portfolio_Forecast.xlsx
+++ b/exports/Ophthalmology_Portfolio_Forecast.xlsx
@@ -19,9 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="398">
-  <si>
-    <t>Viatris EyeCare - Ophthalmology Portfolio Forecast</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="394">
+  <si>
+    <t>Eye Care Franchise - Ophthalmology Portfolio Forecast</t>
   </si>
   <si>
     <t>Sequenzieller Markteintritt DE | 3 Produkte | 7-Jahres-Horizont</t>
@@ -450,7 +450,7 @@
     <t>Tyrvaya (Varenicl.)</t>
   </si>
   <si>
-    <t>Viatris (Oyster Pt.)</t>
+    <t>Specialty Pharma</t>
   </si>
   <si>
     <t>DED, neuer MOA</t>
@@ -477,13 +477,13 @@
     <t>Freier Markt, hohes Volumen</t>
   </si>
   <si>
-    <t>Viatris Ophthalmologie-Pipeline</t>
+    <t>Ophthalmologie-Pipeline (Eye Care Franchise)</t>
   </si>
   <si>
     <t>Strategie</t>
   </si>
   <si>
-    <t>$1B+ Specialty-Umsatz bis 2028 (Viatris Investor Day)</t>
+    <t>Aufbau Specialty-Ophthalmologie durch Akquisitionen + Pipeline</t>
   </si>
   <si>
     <t>Oyster Point Akquisition</t>
@@ -681,7 +681,7 @@
     <t>MVZ-Anteil</t>
   </si>
   <si>
-    <t>Executive Summary - Viatris EyeCare Portfolio</t>
+    <t>Executive Summary - Eye Care Franchise Portfolio</t>
   </si>
   <si>
     <t>Szenario-Vergleich (7-Jahres-Horizont)</t>
@@ -879,7 +879,7 @@
     <t>August 2023 (Phentolamin)</t>
   </si>
   <si>
-    <t>FDA / Viatris IR</t>
+    <t>FDA Public Assessment</t>
   </si>
   <si>
     <t>Tyrvaya FDA-Zulassung</t>
@@ -897,21 +897,18 @@
     <t>Stand Feb. 2025: keine EU-Einreichung</t>
   </si>
   <si>
-    <t>Viatris Pipeline / ClinTrials</t>
-  </si>
-  <si>
-    <t>2023, ~$785M (Viatris)</t>
-  </si>
-  <si>
-    <t>Viatris Investor Relations</t>
+    <t>Pipeline-Daten / ClinTrials</t>
+  </si>
+  <si>
+    <t>2023, ~$785M</t>
+  </si>
+  <si>
+    <t>Oeffentliche Pressemitteilungen</t>
   </si>
   <si>
     <t>2023 erworben (RYZUMVI + MR-141)</t>
   </si>
   <si>
-    <t>Viatris Newsroom</t>
-  </si>
-  <si>
     <t>Presbyopie DE</t>
   </si>
   <si>
@@ -921,15 +918,6 @@
     <t>Epidemiologische Schaetzung</t>
   </si>
   <si>
-    <t>Viatris $1B Specialty Ziel</t>
-  </si>
-  <si>
-    <t>Bis 2028 (Investor Day)</t>
-  </si>
-  <si>
-    <t>Viatris Investor Day 2024</t>
-  </si>
-  <si>
     <t>ANNAHMEN</t>
   </si>
   <si>
@@ -1158,7 +1146,7 @@
     <t>Zeitpunkt und Strategie der EU-Einreichung unklar</t>
   </si>
   <si>
-    <t>Viatris Regulatory Affairs</t>
+    <t>Regulatory Intelligence</t>
   </si>
   <si>
     <t>MR-141 Phase-III Daten</t>
@@ -1167,7 +1155,7 @@
     <t>Ergebnisse Presbyopie-Studie stehen noch aus</t>
   </si>
   <si>
-    <t>ClinicalTrials.gov / Viatris</t>
+    <t>ClinicalTrials.gov</t>
   </si>
   <si>
     <t>AMNOG-Dossier Details</t>
@@ -1233,7 +1221,7 @@
     <t>GKV-SV / Lauer-Taxe Detail</t>
   </si>
   <si>
-    <t>Hinweis: Alle Daten synthetisch. Referenzen: Viatris Investor Relations, FDA/EMA Public Assessments, KBV Aerztestatistik, Grand View Research (Dry Eye), Santen (iKervis), Novaliq (Vevizye), ClinicalTrials.gov. Kein Bezug zu vertraulichen Daten.</t>
+    <t>Hinweis: Alle Daten synthetisch. Referenzen: FDA/EMA Public Assessments, KBV Aerztestatistik, Grand View Research (Dry Eye), Santen (iKervis), Novaliq (Vevizye), ClinicalTrials.gov, oeffentliche Investor Relations. Kein Bezug zu vertraulichen Daten.</t>
   </si>
 </sst>
 </file>
@@ -17133,7 +17121,7 @@
   <sheetPr>
     <tabColor rgb="FF6366F1"/>
   </sheetPr>
-  <dimension ref="B2:E69"/>
+  <dimension ref="B2:E68"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -17395,7 +17383,7 @@
         <v>288</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E24" s="28" t="s">
         <v>243</v>
@@ -17403,63 +17391,63 @@
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>290</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="D25" s="11" t="s">
         <v>291</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>292</v>
       </c>
       <c r="E25" s="28" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="4" t="s">
+    <row r="27" spans="2:5">
+      <c r="B27" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="D28" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E28" s="10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="E26" s="28" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="3" t="s">
+      <c r="C29" s="29" t="s">
         <v>296</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="10" t="s">
+      <c r="D29" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>255</v>
+      <c r="E29" s="29" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C30" s="29" t="s">
         <v>299</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="D30" s="11" t="s">
         <v>300</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>301</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>245</v>
@@ -17467,13 +17455,13 @@
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C31" s="29" t="s">
         <v>302</v>
       </c>
-      <c r="C31" s="29" t="s">
-        <v>303</v>
-      </c>
       <c r="D31" s="11" t="s">
-        <v>304</v>
+        <v>13</v>
       </c>
       <c r="E31" s="29" t="s">
         <v>245</v>
@@ -17481,13 +17469,13 @@
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>305</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>306</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>13</v>
       </c>
       <c r="E32" s="29" t="s">
         <v>245</v>
@@ -17495,13 +17483,13 @@
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C33" s="29" t="s">
         <v>307</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="D33" s="11" t="s">
         <v>308</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>309</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>245</v>
@@ -17509,13 +17497,13 @@
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C34" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="D34" s="11" t="s">
         <v>311</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>312</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>245</v>
@@ -17523,13 +17511,13 @@
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C35" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="D35" s="11" t="s">
         <v>314</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>315</v>
       </c>
       <c r="E35" s="29" t="s">
         <v>245</v>
@@ -17537,13 +17525,13 @@
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C36" s="29" t="s">
         <v>316</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="D36" s="11" t="s">
         <v>317</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>318</v>
       </c>
       <c r="E36" s="29" t="s">
         <v>245</v>
@@ -17551,13 +17539,13 @@
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C37" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="D37" s="11" t="s">
         <v>320</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>321</v>
       </c>
       <c r="E37" s="29" t="s">
         <v>245</v>
@@ -17565,13 +17553,13 @@
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C38" s="29" t="s">
         <v>322</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="D38" s="11" t="s">
         <v>323</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>324</v>
       </c>
       <c r="E38" s="29" t="s">
         <v>245</v>
@@ -17579,13 +17567,13 @@
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C39" s="29" t="s">
         <v>325</v>
       </c>
-      <c r="C39" s="29" t="s">
+      <c r="D39" s="11" t="s">
         <v>326</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>327</v>
       </c>
       <c r="E39" s="29" t="s">
         <v>245</v>
@@ -17593,13 +17581,13 @@
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C40" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="C40" s="29" t="s">
+      <c r="D40" s="11" t="s">
         <v>329</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>330</v>
       </c>
       <c r="E40" s="29" t="s">
         <v>245</v>
@@ -17607,13 +17595,13 @@
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>330</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>331</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>332</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>333</v>
       </c>
       <c r="E41" s="29" t="s">
         <v>245</v>
@@ -17621,63 +17609,63 @@
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E42" s="29" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="43" spans="2:5">
-      <c r="B43" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C43" s="29" t="s">
+    <row r="44" spans="2:5">
+      <c r="B44" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D45" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E43" s="29" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5">
-      <c r="B45" s="3" t="s">
+      <c r="E45" s="10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="35" customHeight="1">
+      <c r="B46" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="2:5">
-      <c r="B46" s="10" t="s">
+      <c r="C46" s="30" t="s">
         <v>339</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="D46" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>255</v>
+      <c r="E46" s="30" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="35" customHeight="1">
       <c r="B47" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C47" s="30" t="s">
         <v>342</v>
       </c>
-      <c r="C47" s="30" t="s">
+      <c r="D47" s="11" t="s">
         <v>343</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>344</v>
       </c>
       <c r="E47" s="30" t="s">
         <v>247</v>
@@ -17685,13 +17673,13 @@
     </row>
     <row r="48" spans="2:5" ht="35" customHeight="1">
       <c r="B48" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C48" s="30" t="s">
         <v>345</v>
       </c>
-      <c r="C48" s="30" t="s">
+      <c r="D48" s="11" t="s">
         <v>346</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>347</v>
       </c>
       <c r="E48" s="30" t="s">
         <v>247</v>
@@ -17699,13 +17687,13 @@
     </row>
     <row r="49" spans="2:5" ht="35" customHeight="1">
       <c r="B49" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C49" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="C49" s="30" t="s">
+      <c r="D49" s="11" t="s">
         <v>349</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>350</v>
       </c>
       <c r="E49" s="30" t="s">
         <v>247</v>
@@ -17713,13 +17701,13 @@
     </row>
     <row r="50" spans="2:5" ht="35" customHeight="1">
       <c r="B50" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C50" s="30" t="s">
         <v>351</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="D50" s="11" t="s">
         <v>352</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>353</v>
       </c>
       <c r="E50" s="30" t="s">
         <v>247</v>
@@ -17727,13 +17715,13 @@
     </row>
     <row r="51" spans="2:5" ht="35" customHeight="1">
       <c r="B51" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C51" s="30" t="s">
         <v>354</v>
       </c>
-      <c r="C51" s="30" t="s">
+      <c r="D51" s="11" t="s">
         <v>355</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>356</v>
       </c>
       <c r="E51" s="30" t="s">
         <v>247</v>
@@ -17741,13 +17729,13 @@
     </row>
     <row r="52" spans="2:5" ht="35" customHeight="1">
       <c r="B52" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C52" s="30" t="s">
         <v>357</v>
       </c>
-      <c r="C52" s="30" t="s">
+      <c r="D52" s="11" t="s">
         <v>358</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>359</v>
       </c>
       <c r="E52" s="30" t="s">
         <v>247</v>
@@ -17755,63 +17743,63 @@
     </row>
     <row r="53" spans="2:5" ht="35" customHeight="1">
       <c r="B53" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="C53" s="30" t="s">
         <v>360</v>
       </c>
-      <c r="C53" s="30" t="s">
+      <c r="D53" s="11" t="s">
         <v>361</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>362</v>
       </c>
       <c r="E53" s="30" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="54" spans="2:5" ht="35" customHeight="1">
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="2:5">
+      <c r="B55" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="2:5">
+      <c r="B56" s="10" t="s">
         <v>363</v>
       </c>
-      <c r="C54" s="30" t="s">
+      <c r="C56" s="10" t="s">
         <v>364</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="D56" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="E54" s="30" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5">
-      <c r="B56" s="3" t="s">
+      <c r="E56" s="10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="2:5">
-      <c r="B57" s="10" t="s">
+      <c r="C57" s="31" t="s">
         <v>367</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="D57" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="D57" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>255</v>
+      <c r="E57" s="31" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="58" spans="2:5">
       <c r="B58" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C58" s="31" t="s">
         <v>370</v>
       </c>
-      <c r="C58" s="31" t="s">
+      <c r="D58" s="11" t="s">
         <v>371</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>372</v>
       </c>
       <c r="E58" s="31" t="s">
         <v>249</v>
@@ -17819,13 +17807,13 @@
     </row>
     <row r="59" spans="2:5">
       <c r="B59" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C59" s="31" t="s">
         <v>373</v>
       </c>
-      <c r="C59" s="31" t="s">
+      <c r="D59" s="11" t="s">
         <v>374</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>375</v>
       </c>
       <c r="E59" s="31" t="s">
         <v>249</v>
@@ -17833,13 +17821,13 @@
     </row>
     <row r="60" spans="2:5">
       <c r="B60" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="C60" s="31" t="s">
         <v>376</v>
       </c>
-      <c r="C60" s="31" t="s">
+      <c r="D60" s="11" t="s">
         <v>377</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>378</v>
       </c>
       <c r="E60" s="31" t="s">
         <v>249</v>
@@ -17847,13 +17835,13 @@
     </row>
     <row r="61" spans="2:5">
       <c r="B61" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="C61" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C61" s="31" t="s">
+      <c r="D61" s="11" t="s">
         <v>380</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>381</v>
       </c>
       <c r="E61" s="31" t="s">
         <v>249</v>
@@ -17861,13 +17849,13 @@
     </row>
     <row r="62" spans="2:5">
       <c r="B62" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C62" s="31" t="s">
         <v>382</v>
       </c>
-      <c r="C62" s="31" t="s">
+      <c r="D62" s="11" t="s">
         <v>383</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>384</v>
       </c>
       <c r="E62" s="31" t="s">
         <v>249</v>
@@ -17875,13 +17863,13 @@
     </row>
     <row r="63" spans="2:5">
       <c r="B63" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="C63" s="31" t="s">
         <v>385</v>
       </c>
-      <c r="C63" s="31" t="s">
+      <c r="D63" s="11" t="s">
         <v>386</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>387</v>
       </c>
       <c r="E63" s="31" t="s">
         <v>249</v>
@@ -17889,13 +17877,13 @@
     </row>
     <row r="64" spans="2:5">
       <c r="B64" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="C64" s="31" t="s">
         <v>388</v>
       </c>
-      <c r="C64" s="31" t="s">
+      <c r="D64" s="11" t="s">
         <v>389</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>390</v>
       </c>
       <c r="E64" s="31" t="s">
         <v>249</v>
@@ -17903,49 +17891,35 @@
     </row>
     <row r="65" spans="2:5">
       <c r="B65" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="C65" s="31" t="s">
         <v>391</v>
       </c>
-      <c r="C65" s="31" t="s">
+      <c r="D65" s="11" t="s">
         <v>392</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>393</v>
       </c>
       <c r="E65" s="31" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="66" spans="2:5">
-      <c r="B66" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="C66" s="31" t="s">
-        <v>395</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>396</v>
-      </c>
-      <c r="E66" s="31" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5">
-      <c r="B69" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
+    <row r="68" spans="2:5">
+      <c r="B68" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B68:E68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>